<commit_message>
planning et journal de travail
31.03/11h45
</commit_message>
<xml_diff>
--- a/journal de travail.xlsx
+++ b/journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\133_Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99270330-F337-48D4-A1B5-70AB0CCE4E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620641FE-FA8E-4F16-A42C-F3AED9A911FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67ED1187-3756-426A-A904-E9527551CCF3}"/>
+    <workbookView xWindow="-11655" yWindow="5970" windowWidth="21600" windowHeight="11385" xr2:uid="{67ED1187-3756-426A-A904-E9527551CCF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -52,12 +52,30 @@
   <si>
     <t>Tâches</t>
   </si>
+  <si>
+    <t>Gestion de projet : Planning</t>
+  </si>
+  <si>
+    <t>Analyse : Use Case Globale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse : Use Case Client / Rest Client </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse : Use Case Admin / Rest Admin </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Analyse : Use Case API Gateway</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +101,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -228,6 +261,17 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -237,21 +281,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -261,21 +290,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -592,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAA8B3-4558-49E4-B202-A0E376610493}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,346 +651,395 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="1">
         <v>45016</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="A4" s="4">
+        <v>45016</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+      <c r="A5" s="4">
+        <v>45016</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
+      <c r="A6" s="4">
+        <v>45016</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="13"/>
       <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="15">
+        <f>SUM(C3:C55)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D56" s="15">
+        <f>SUM(D3:D55)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>